<commit_message>
major changes in loader logic and notes
</commit_message>
<xml_diff>
--- a/data/sample_survey3.xlsx
+++ b/data/sample_survey3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shmuc\Desktop\Thesis Project\Thesis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EAB0F7C7-DB66-44E0-90F8-277275ADD82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{773474AB-FD06-49A2-A987-9DB1E8DB36A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{8F41F115-760D-475F-A656-C62DA987F20C}"/>
+    <workbookView xWindow="5400" yWindow="0" windowWidth="16200" windowHeight="9307" xr2:uid="{8F41F115-760D-475F-A656-C62DA987F20C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,6 +445,11 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="15.06640625" customWidth="1"/>
+    <col min="2" max="2" width="30.59765625" customWidth="1"/>
+    <col min="3" max="3" width="22.06640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">

</xml_diff>